<commit_message>
Started working on Rtreedist
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="10800"/>
+    <workbookView xWindow="120" yWindow="96" windowWidth="12432" windowHeight="10800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="phylip-programs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>clique.exe</t>
   </si>
@@ -207,13 +207,37 @@
   </si>
   <si>
     <t>Warns before overwriting files.</t>
+  </si>
+  <si>
+    <t>threshml.exe*</t>
+  </si>
+  <si>
+    <t>Rthreshml</t>
+  </si>
+  <si>
+    <t>write.continuous</t>
+  </si>
+  <si>
+    <t>Writes continuous character data in the format of contrast.</t>
+  </si>
+  <si>
+    <t>to.integers</t>
+  </si>
+  <si>
+    <t>Converts factor or character to integers 0, 1, 2, etc. For Rthreshml.</t>
+  </si>
+  <si>
+    <t>crop</t>
+  </si>
+  <si>
+    <t>Crops a vector of strings to the set of first characters.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -749,6 +773,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -827,6 +856,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -861,6 +891,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1036,22 +1067,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -1062,17 +1095,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1084,7 +1117,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1096,22 +1129,22 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1123,7 +1156,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1135,12 +1168,12 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1152,62 +1185,62 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1219,58 +1252,69 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="3">
+        <v>41613</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1281,23 +1325,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="77.88671875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1311,7 +1355,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -1325,7 +1369,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -1339,7 +1383,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -1353,7 +1397,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>54</v>
       </c>
@@ -1367,7 +1411,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -1381,7 +1425,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>58</v>
       </c>
@@ -1395,7 +1439,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>60</v>
       </c>
@@ -1409,7 +1453,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>62</v>
       </c>
@@ -1421,6 +1465,48 @@
       </c>
       <c r="D9" s="2" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="3">
+        <v>41613</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="3">
+        <v>41613</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="3">
+        <v>41613</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New man pages & other updates. New build.
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="96" windowWidth="12432" windowHeight="10800" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="phylip-programs" sheetId="1" r:id="rId1"/>
     <sheet name="addt'l-functions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>clique.exe</t>
   </si>
@@ -231,13 +231,16 @@
   </si>
   <si>
     <t>Crops a vector of strings to the set of first characters.</t>
+  </si>
+  <si>
+    <t>Rtreedist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -856,7 +859,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -891,7 +893,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1067,24 +1068,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -1095,17 +1096,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1118,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1129,22 +1130,22 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1156,7 +1157,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1168,12 +1169,12 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1185,62 +1186,62 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1252,57 +1253,57 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
         <v>64</v>
       </c>
@@ -1313,9 +1314,15 @@
         <v>41613</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="3">
+        <v>41613</v>
       </c>
     </row>
   </sheetData>
@@ -1325,23 +1332,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="77.88671875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="77.85546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1355,7 +1362,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -1369,7 +1376,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -1383,7 +1390,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -1397,7 +1404,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>54</v>
       </c>
@@ -1411,7 +1418,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -1425,7 +1432,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>58</v>
       </c>
@@ -1439,7 +1446,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>60</v>
       </c>
@@ -1453,7 +1460,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>62</v>
       </c>
@@ -1467,7 +1474,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>66</v>
       </c>
@@ -1481,7 +1488,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
@@ -1495,7 +1502,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
New functions to handle aa sequences
New functions for protein sequences. Some other stuff.
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="10800"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="10800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="phylip-programs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
   <si>
     <t>clique.exe</t>
   </si>
@@ -243,6 +243,36 @@
   </si>
   <si>
     <t>Rconsense</t>
+  </si>
+  <si>
+    <t>Rproml</t>
+  </si>
+  <si>
+    <t>Rpromlk/Rproml(…,clock=TRUE)**</t>
+  </si>
+  <si>
+    <t>*not in PHYLIP 3.695</t>
+  </si>
+  <si>
+    <t>**does not appear to work, but this seems to be due to promlk - not the wrapper. A tree is returned, but all branch lengths are 0.</t>
+  </si>
+  <si>
+    <t>as.protseq</t>
+  </si>
+  <si>
+    <t>Converts phyDat to protseq object.</t>
+  </si>
+  <si>
+    <t>read.protein</t>
+  </si>
+  <si>
+    <t>Read protein sequence from file in fasta or "sequential" format.</t>
+  </si>
+  <si>
+    <t>print.protseq</t>
+  </si>
+  <si>
+    <t>S3 generic print method for objects of class "protseq".</t>
   </si>
 </sst>
 </file>
@@ -1078,16 +1108,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -1294,11 +1324,23 @@
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="B27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="3">
+        <v>41617</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="B28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="3">
+        <v>41617</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
@@ -1350,6 +1392,16 @@
       </c>
       <c r="C36" s="3">
         <v>41613</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1360,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1543,6 +1595,48 @@
         <v>71</v>
       </c>
     </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="3">
+        <v>41617</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="3">
+        <v>41617</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="3">
+        <v>41617</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rprotdist & updates to .Rd files
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="88">
   <si>
     <t>clique.exe</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>Rprotpars</t>
+  </si>
+  <si>
+    <t>Rprotdist</t>
   </si>
 </sst>
 </file>
@@ -1115,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1350,6 +1353,12 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="3">
+        <v>41622</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
New functions to set the path to PHYLIP exe
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="96" windowWidth="12432" windowHeight="10800"/>
+    <workbookView xWindow="120" yWindow="96" windowWidth="12432" windowHeight="10800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="phylip-programs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
   <si>
     <t>clique.exe</t>
   </si>
@@ -291,6 +291,18 @@
   </si>
   <si>
     <t>***functional, but incomplete</t>
+  </si>
+  <si>
+    <t>setPath</t>
+  </si>
+  <si>
+    <t>Sets path to the folder containing PHYLIP executables for current R session.</t>
+  </si>
+  <si>
+    <t>clearPath</t>
+  </si>
+  <si>
+    <t>Clears path to PHYLIP executables.</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1467,9 +1479,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1692,6 +1704,34 @@
         <v>88</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="3">
+        <v>41629</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="3">
+        <v>41629</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New functions Rmix & Rpenny
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="96" windowWidth="12432" windowHeight="10800" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="96" windowWidth="12432" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="phylip-programs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
   <si>
     <t>clique.exe</t>
   </si>
@@ -303,6 +303,15 @@
   </si>
   <si>
     <t>Clears path to PHYLIP executables.</t>
+  </si>
+  <si>
+    <t>Rpars</t>
+  </si>
+  <si>
+    <t>Rmix</t>
+  </si>
+  <si>
+    <t>Rpenny</t>
   </si>
 </sst>
 </file>
@@ -1142,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1342,6 +1351,12 @@
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="3">
+        <v>41638</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
@@ -1364,10 +1379,22 @@
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="3">
+        <v>41634</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="3">
+        <v>41638</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1481,7 +1508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New function Rdollop & doc.
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="100">
   <si>
     <t>clique.exe</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>Rpenny</t>
+  </si>
+  <si>
+    <t>Rdollop</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1155,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1304,6 +1307,12 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="3">
+        <v>41686</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
New function Rdolpenny & doc.
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="101">
   <si>
     <t>clique.exe</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>Rdollop</t>
+  </si>
+  <si>
+    <t>Rdolpenny</t>
   </si>
 </sst>
 </file>
@@ -1154,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1323,6 +1326,12 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="3">
+        <v>41687</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
New function Rgendist & doc.
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="96" windowWidth="12432" windowHeight="10800"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="10800"/>
   </bookViews>
   <sheets>
     <sheet name="phylip-programs" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
   <si>
     <t>clique.exe</t>
   </si>
@@ -318,13 +318,16 @@
   </si>
   <si>
     <t>Rdolpenny</t>
+  </si>
+  <si>
+    <t>Rgendist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -943,7 +946,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -978,7 +980,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1154,24 +1155,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -1182,12 +1183,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1198,7 +1199,7 @@
         <v>41616</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1210,7 +1211,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1222,7 +1223,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1233,7 +1234,7 @@
         <v>41624</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1244,7 +1245,7 @@
         <v>41615</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1255,7 +1256,7 @@
         <v>41627</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1267,7 +1268,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1279,12 +1280,12 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1296,7 +1297,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1307,7 +1308,7 @@
         <v>41615</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1318,12 +1319,12 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1334,17 +1335,17 @@
         <v>41687</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1355,17 +1356,23 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="3">
+        <v>41688</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1376,12 +1383,12 @@
         <v>41638</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1393,7 +1400,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1404,7 +1411,7 @@
         <v>41634</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1415,7 +1422,7 @@
         <v>41638</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -1426,7 +1433,7 @@
         <v>41617</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1437,7 +1444,7 @@
         <v>41617</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -1448,7 +1455,7 @@
         <v>41622</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -1459,27 +1466,27 @@
         <v>41622</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
         <v>64</v>
       </c>
@@ -1490,7 +1497,7 @@
         <v>41613</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
@@ -1501,17 +1508,17 @@
         <v>41613</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
         <v>91</v>
       </c>
@@ -1523,23 +1530,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="77.88671875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="77.85546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1553,7 +1560,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
@@ -1567,7 +1574,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>52</v>
       </c>
@@ -1581,7 +1588,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>94</v>
       </c>
@@ -1595,7 +1602,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>70</v>
       </c>
@@ -1609,7 +1616,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>62</v>
       </c>
@@ -1623,7 +1630,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
@@ -1637,7 +1644,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -1651,7 +1658,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>60</v>
       </c>
@@ -1665,7 +1672,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>85</v>
       </c>
@@ -1679,7 +1686,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>80</v>
       </c>
@@ -1693,7 +1700,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>92</v>
       </c>
@@ -1707,7 +1714,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>54</v>
       </c>
@@ -1721,7 +1728,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>68</v>
       </c>
@@ -1735,7 +1742,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
@@ -1749,7 +1756,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>56</v>
       </c>
@@ -1763,7 +1770,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Working on Rrestdist; new class "rest.dist".
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="10800"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="10800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="phylip-programs" sheetId="1" r:id="rId1"/>
@@ -1161,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1542,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1585,156 +1585,156 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="B3" s="3">
-        <v>41610</v>
+        <v>41629</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3">
-        <v>41629</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>41609</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3">
-        <v>41613</v>
+        <v>41617</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B6" s="3">
-        <v>41608</v>
+        <v>41617</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B7" s="3">
-        <v>41610</v>
+        <v>41629</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B8" s="3">
-        <v>41609</v>
-      </c>
-      <c r="C8" s="3" t="s">
+        <v>41610</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B9" s="3">
-        <v>41609</v>
+        <v>41610</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3">
-        <v>41617</v>
+        <v>41613</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B11" s="3">
-        <v>41617</v>
+        <v>41608</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="B12" s="3">
-        <v>41629</v>
+        <v>41610</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B13" s="3">
-        <v>41610</v>
+        <v>41609</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1795,7 +1795,7 @@
     </row>
   </sheetData>
   <sortState ref="A2:D17">
-    <sortCondition ref="A2:A17"/>
+    <sortCondition ref="C2:C17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished Rclique, Rrestml, & doc
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="112">
   <si>
     <t>clique.exe</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>Rrestdist</t>
+  </si>
+  <si>
+    <t>Rrestml</t>
+  </si>
+  <si>
+    <t>Rclique</t>
   </si>
 </sst>
 </file>
@@ -1182,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1211,6 +1217,12 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="3">
+        <v>41695</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
@@ -1510,6 +1522,12 @@
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="3">
+        <v>41695</v>
       </c>
     </row>
     <row r="33" spans="1:3">

</xml_diff>

<commit_message>
Some updates to submit to CRAN
Fingers crossed :)
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12435" windowHeight="10800"/>
+    <workbookView xWindow="120" yWindow="96" windowWidth="12432" windowHeight="10800" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="phylip-programs" sheetId="1" r:id="rId1"/>
     <sheet name="addt'l-functions" sheetId="2" r:id="rId2"/>
+    <sheet name="importFrom-ape" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
   <si>
     <t>clique.exe</t>
   </si>
@@ -351,13 +352,31 @@
   </si>
   <si>
     <t>Rclique</t>
+  </si>
+  <si>
+    <t>read.tree</t>
+  </si>
+  <si>
+    <t>write.tree</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>unroot</t>
+  </si>
+  <si>
+    <t>is.binary.tree</t>
+  </si>
+  <si>
+    <t>multi2di</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -976,6 +995,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1010,6 +1030,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1185,24 +1206,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -1213,7 +1234,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1224,7 +1245,7 @@
         <v>41695</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1235,7 +1256,7 @@
         <v>41616</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1247,7 +1268,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1259,7 +1280,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1270,7 +1291,7 @@
         <v>41624</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1281,7 +1302,7 @@
         <v>41615</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1292,7 +1313,7 @@
         <v>41627</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1304,7 +1325,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1316,12 +1337,12 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1333,7 +1354,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1344,7 +1365,7 @@
         <v>41615</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1355,12 +1376,12 @@
         <v>41686</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1371,17 +1392,17 @@
         <v>41687</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1392,7 +1413,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1403,7 +1424,7 @@
         <v>41688</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1414,7 +1435,7 @@
         <v>41689</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1425,12 +1446,12 @@
         <v>41638</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1442,7 +1463,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1453,7 +1474,7 @@
         <v>41634</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1464,7 +1485,7 @@
         <v>41638</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -1475,7 +1496,7 @@
         <v>41617</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1486,7 +1507,7 @@
         <v>41617</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -1497,7 +1518,7 @@
         <v>41622</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -1508,7 +1529,7 @@
         <v>41622</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -1519,7 +1540,7 @@
         <v>41691</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1530,17 +1551,17 @@
         <v>41695</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>64</v>
       </c>
@@ -1551,7 +1572,7 @@
         <v>41613</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
@@ -1562,17 +1583,17 @@
         <v>41613</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>91</v>
       </c>
@@ -1584,23 +1605,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="77.88671875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -1614,7 +1635,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
@@ -1628,7 +1649,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>94</v>
       </c>
@@ -1642,7 +1663,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -1656,7 +1677,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
@@ -1670,7 +1691,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>80</v>
       </c>
@@ -1684,7 +1705,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>92</v>
       </c>
@@ -1698,7 +1719,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -1712,7 +1733,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -1726,7 +1747,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>70</v>
       </c>
@@ -1740,7 +1761,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>62</v>
       </c>
@@ -1754,7 +1775,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -1768,7 +1789,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>60</v>
       </c>
@@ -1782,7 +1803,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>68</v>
       </c>
@@ -1796,7 +1817,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>66</v>
       </c>
@@ -1810,7 +1831,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>56</v>
       </c>
@@ -1824,7 +1845,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
@@ -1838,7 +1859,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>103</v>
       </c>
@@ -1852,7 +1873,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>105</v>
       </c>
@@ -1866,7 +1887,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>107</v>
       </c>
@@ -1886,4 +1907,49 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rseqboot done (for now)
</commit_message>
<xml_diff>
--- a/Rphylip.work-list.xlsx
+++ b/Rphylip.work-list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
   <si>
     <t>clique.exe</t>
   </si>
@@ -370,6 +370,39 @@
   </si>
   <si>
     <t>multi2di</t>
+  </si>
+  <si>
+    <t>Rseqboot</t>
+  </si>
+  <si>
+    <t>read.multi.dna</t>
+  </si>
+  <si>
+    <t>Reads multiple DNA datasets from file.</t>
+  </si>
+  <si>
+    <t>read.multi.phylip.data</t>
+  </si>
+  <si>
+    <t>Reads multiple phylip.data datasets from file.</t>
+  </si>
+  <si>
+    <t>read.multi.rest.data</t>
+  </si>
+  <si>
+    <t>Reads multiple rest.data datasets from file.</t>
+  </si>
+  <si>
+    <t>read.phylip.data</t>
+  </si>
+  <si>
+    <t>Reads phylip.data.</t>
+  </si>
+  <si>
+    <t>read.rest.data</t>
+  </si>
+  <si>
+    <t>Reads rest.data.</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1241,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1558,6 +1591,12 @@
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="B34" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="3">
+        <v>41723</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
@@ -1604,15 +1643,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="77.85546875" style="2" customWidth="1"/>
@@ -1897,6 +1934,76 @@
       </c>
       <c r="D20" s="2" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="3">
+        <v>41723</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="3">
+        <v>41723</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="3">
+        <v>41723</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="3">
+        <v>41723</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="3">
+        <v>41723</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>